<commit_message>
added new by tesa
</commit_message>
<xml_diff>
--- a/Data Files/ecommerce data binding.xlsx
+++ b/Data Files/ecommerce data binding.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="sign up" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="shopping electronics" sheetId="3" r:id="rId3"/>
+    <sheet name="shopping baju" sheetId="4" r:id="rId4"/>
+    <sheet name="shopping sofa" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>nama</t>
   </si>
@@ -36,16 +40,31 @@
   <si>
     <t>16amberegul</t>
   </si>
+  <si>
+    <t>resendemail</t>
+  </si>
+  <si>
+    <t>handphone</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>baju</t>
+  </si>
+  <si>
+    <t>sofa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -58,11 +77,18 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -76,7 +102,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -84,29 +126,60 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,38 +193,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,38 +217,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -206,13 +225,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,19 +246,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,19 +366,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,139 +390,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,22 +449,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,21 +475,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,163 +520,183 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -693,10 +706,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1020,42 +1042,42 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="27.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.4444444444444" style="1" customWidth="1"/>
-    <col min="3" max="4" width="27.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.3333333333333" style="6" customWidth="1"/>
+    <col min="2" max="2" width="34.4444444444444" style="6" customWidth="1"/>
+    <col min="3" max="4" width="27.3333333333333" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1066,4 +1088,140 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="3" width="32.6666666666667" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="rezamuhammadsaput@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="rezamuhammadsaput@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="12.8888888888889" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="8.88888888888889" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="8.88888888888889" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>